<commit_message>
FunbitrageParameterBacktestBothWays 파일에 12% 상승 돌파 시 perpetual long, delivery short 백테스트 해봄
</commit_message>
<xml_diff>
--- a/GPT용3.xlsx
+++ b/GPT용3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\world\PycharmProjects\Funbitrage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FB6AB4-BBBD-449C-8E3A-81C550E42E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D49CBC-0934-4A3F-8F01-B4205336C23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="3765" windowWidth="21600" windowHeight="11295" xr2:uid="{594C5422-4EB6-409A-9828-F96DC8DC59F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{594C5422-4EB6-409A-9828-F96DC8DC59F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -192,7 +192,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -207,9 +207,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -12869,7 +12866,7 @@
   <dimension ref="A1:E2893"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12906,7 +12903,7 @@
       <c r="C2" s="5">
         <v>69352.399999999994</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="4">
@@ -12925,7 +12922,7 @@
       <c r="C3" s="5">
         <v>70942.7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="4">
@@ -12944,7 +12941,7 @@
       <c r="C4" s="5">
         <v>69331.600000000006</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="4">
@@ -12963,7 +12960,7 @@
       <c r="C5" s="5">
         <v>69911.199999999997</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="4">
@@ -12982,7 +12979,7 @@
       <c r="C6" s="5">
         <v>69879.7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="4">
@@ -13001,7 +12998,7 @@
       <c r="C7" s="5">
         <v>71686.8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4">
@@ -13020,7 +13017,7 @@
       <c r="C8" s="5">
         <v>70799</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="4">
@@ -13039,7 +13036,7 @@
       <c r="C9" s="5">
         <v>70893.8</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="4">
@@ -13058,7 +13055,7 @@
       <c r="C10" s="5">
         <v>69674.2</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="4">
@@ -13077,7 +13074,7 @@
       <c r="C11" s="5">
         <v>69963.3</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="4">
@@ -13096,7 +13093,7 @@
       <c r="C12" s="5">
         <v>69445</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="4">
@@ -13115,7 +13112,7 @@
       <c r="C13" s="5">
         <v>68895</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="4">
@@ -13134,7 +13131,7 @@
       <c r="C14" s="5">
         <v>65336.5</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="4">
@@ -13153,7 +13150,7 @@
       <c r="C15" s="5">
         <v>65673.100000000006</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="4">
@@ -13172,7 +13169,7 @@
       <c r="C16" s="5">
         <v>64906.3</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="4">
@@ -13191,7 +13188,7 @@
       <c r="C17" s="5">
         <v>62437.2</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="4">
@@ -13210,7 +13207,7 @@
       <c r="C18" s="5">
         <v>62824</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="4">
@@ -13229,7 +13226,7 @@
       <c r="C19" s="5">
         <v>64493.5</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="4">
@@ -13248,7 +13245,7 @@
       <c r="C20" s="5">
         <v>64581.1</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="4">
@@ -13267,7 +13264,7 @@
       <c r="C21" s="5">
         <v>65305</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E21" s="4">
@@ -13286,7 +13283,7 @@
       <c r="C22" s="5">
         <v>64350</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="4">
@@ -13305,7 +13302,7 @@
       <c r="C23" s="5">
         <v>64349.9</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="4">
@@ -13324,7 +13321,7 @@
       <c r="C24" s="5">
         <v>62940.3</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="4">
@@ -13343,7 +13340,7 @@
       <c r="C25" s="5">
         <v>62778.2</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="4">
@@ -13362,7 +13359,7 @@
       <c r="C26" s="5">
         <v>62895.8</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="4">
@@ -13381,7 +13378,7 @@
       <c r="C27" s="5">
         <v>65620</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="4">
@@ -13400,7 +13397,7 @@
       <c r="C28" s="5">
         <v>68912.5</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="4">
@@ -13419,7 +13416,7 @@
       <c r="C29" s="5">
         <v>69153.600000000006</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="4">

</xml_diff>